<commit_message>
Leaderboard with best score
</commit_message>
<xml_diff>
--- a/docs/assignment/grading_full.xlsx
+++ b/docs/assignment/grading_full.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="176">
   <si>
     <t>Grading Data</t>
   </si>
@@ -67,6 +67,18 @@
     <t>[50.36, 10.33, 9.62]</t>
   </si>
   <si>
+    <t>Rimski_Korsako</t>
+  </si>
+  <si>
+    <t>[93.06, 12.61, 12.53]</t>
+  </si>
+  <si>
+    <t>[95.12, 11.68, 11.76]</t>
+  </si>
+  <si>
+    <t>[91.96, 10.83, 10.66]</t>
+  </si>
+  <si>
     <t xml:space="preserve">Malkarenn     </t>
   </si>
   <si>
@@ -109,13 +121,13 @@
     <t>[[True, True, True, True, True], [True, True, True, True, True], [False, True, True, True, True]]</t>
   </si>
   <si>
-    <t>[67.37, 9.38, 9.37]</t>
-  </si>
-  <si>
-    <t>[77.21, 9.66, 8.5]</t>
-  </si>
-  <si>
-    <t>[56.56, 7.66, 7.58]</t>
+    <t>[67.98, 9.33, 9.32]</t>
+  </si>
+  <si>
+    <t>[105.38, 8.35, 8.36]</t>
+  </si>
+  <si>
+    <t>[56.62, 7.9, 7.89]</t>
   </si>
   <si>
     <t xml:space="preserve">pizza         </t>
@@ -133,12 +145,24 @@
     <t>[64.02, 7.78, 7.66]</t>
   </si>
   <si>
+    <t xml:space="preserve">tau           </t>
+  </si>
+  <si>
+    <t>[[True, True, True, True, True], [True, False, True, True, True], [True, True, True, True, True]]</t>
+  </si>
+  <si>
+    <t>[44.54, 10.94, 10.93]</t>
+  </si>
+  <si>
+    <t>[44.46, 10.85, 10.85]</t>
+  </si>
+  <si>
+    <t>[47.29, 10.74, 10.76]</t>
+  </si>
+  <si>
     <t>my_assignment.</t>
   </si>
   <si>
-    <t>[[True, True, True, True, True], [True, False, True, True, True], [True, True, True, True, True]]</t>
-  </si>
-  <si>
     <t>[49.78, 12.23, 12.13]</t>
   </si>
   <si>
@@ -166,24 +190,21 @@
     <t xml:space="preserve">THURGOVIA     </t>
   </si>
   <si>
-    <t>[[True, True, True, True, True], [True, True, True, True, True], [True, True, True, False, False]]</t>
-  </si>
-  <si>
-    <t>[53.99, 12.23, 12.04]</t>
-  </si>
-  <si>
-    <t>[52.88, 11.75, 11.5]</t>
-  </si>
-  <si>
-    <t>[46.04, 11.01, 11.26]</t>
+    <t>[[True, True, True, True, True], [True, True, True, True, False], [True, True, True, True, False]]</t>
+  </si>
+  <si>
+    <t>[52.15, 11.44, 11.03]</t>
+  </si>
+  <si>
+    <t>[51.03, 10.74, 10.38]</t>
+  </si>
+  <si>
+    <t>[43.06, 9.54, 9.63]</t>
   </si>
   <si>
     <t xml:space="preserve">AGN_v1        </t>
   </si>
   <si>
-    <t>[[True, True, True, True, True], [True, True, True, True, False], [True, True, True, True, False]]</t>
-  </si>
-  <si>
     <t>[48.35, 13.01, 13.02]</t>
   </si>
   <si>
@@ -241,6 +262,36 @@
     <t>[72.82, 10.66, 10.75]</t>
   </si>
   <si>
+    <t xml:space="preserve">odermatt      </t>
+  </si>
+  <si>
+    <t>[[True, True, True, True, True], [True, True, False, True, True], [True, True, False, True, False]]</t>
+  </si>
+  <si>
+    <t>[25.87, 12.49, 12.41]</t>
+  </si>
+  <si>
+    <t>[24.13, 11.85, 11.73]</t>
+  </si>
+  <si>
+    <t>[23.9, 11.37, 11.78]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CPT           </t>
+  </si>
+  <si>
+    <t>[[True, True, True, True, True], [True, False, True, True, True], [True, False, False, True, False]]</t>
+  </si>
+  <si>
+    <t>[84.28, 9.42, 8.78]</t>
+  </si>
+  <si>
+    <t>[75.18, 8.57, 8.34]</t>
+  </si>
+  <si>
+    <t>[71.4, 8.02, 7.28]</t>
+  </si>
+  <si>
     <t>TrackTouristV2</t>
   </si>
   <si>
@@ -325,54 +376,27 @@
     <t>[58.98, 11.23, 11.23]</t>
   </si>
   <si>
-    <t>Rimski_Korsako</t>
-  </si>
-  <si>
-    <t>[[True, True, True, True, False], [False, False, False, False, False], [False, False, False, False, False]]</t>
-  </si>
-  <si>
-    <t>[103.87, 11.0, 10.96]</t>
-  </si>
-  <si>
-    <t>[106.26, 10.14, 10.23]</t>
+    <t xml:space="preserve">Oscar_F_V2    </t>
+  </si>
+  <si>
+    <t>[[True, False, True, True, True], [False, True, True, True, False], [False, True, True, True, False]]</t>
+  </si>
+  <si>
+    <t>[[True, True, True, True, True], [False, True, False, True, True], [True, True, False, True, True]]</t>
+  </si>
+  <si>
+    <t>[[True, True, True, True, True], [False, False, False, False, False], [False, False, False, False, False]]</t>
+  </si>
+  <si>
+    <t>[71.9, 33.86, 19.21]</t>
+  </si>
+  <si>
+    <t>[47.3, 17.47, 19.14]</t>
   </si>
   <si>
     <t>[1000.0, 1000.0, 1000.0]</t>
   </si>
   <si>
-    <t xml:space="preserve">Oscar_F_V2    </t>
-  </si>
-  <si>
-    <t>[[True, False, True, True, True], [False, True, True, True, False], [False, True, True, True, False]]</t>
-  </si>
-  <si>
-    <t>[[True, True, True, True, True], [False, True, False, True, True], [True, True, False, True, True]]</t>
-  </si>
-  <si>
-    <t>[[True, True, True, True, True], [False, False, False, False, False], [False, False, False, False, False]]</t>
-  </si>
-  <si>
-    <t>[71.9, 33.86, 19.21]</t>
-  </si>
-  <si>
-    <t>[47.3, 17.47, 19.14]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tau           </t>
-  </si>
-  <si>
-    <t>[[False, True, False, True, True], [False, True, False, True, True], [True, True, False, True, True]]</t>
-  </si>
-  <si>
-    <t>[44.91, 10.94, 10.92]</t>
-  </si>
-  <si>
-    <t>[44.64, 10.84, 10.86]</t>
-  </si>
-  <si>
-    <t>[45.74, 10.79, 10.8]</t>
-  </si>
-  <si>
     <t xml:space="preserve">mmm128        </t>
   </si>
   <si>
@@ -406,18 +430,6 @@
     <t>[129.71, 14.89, 14.45]</t>
   </si>
   <si>
-    <t xml:space="preserve">CPT           </t>
-  </si>
-  <si>
-    <t>[[True, True, True, True, True], [True, False, True, True, True], [True, False, False, True, False]]</t>
-  </si>
-  <si>
-    <t>[82.82, 9.43, 8.82]</t>
-  </si>
-  <si>
-    <t>[91.33, 8.56, 8.33]</t>
-  </si>
-  <si>
     <t xml:space="preserve">slowking      </t>
   </si>
   <si>
@@ -454,45 +466,33 @@
     <t>[86.1, 12.69, 12.62]</t>
   </si>
   <si>
-    <t xml:space="preserve">odermatt      </t>
-  </si>
-  <si>
-    <t>[[True, True, True, True, True], [False, True, False, True, True], [False, True, False, True, True]]</t>
+    <t xml:space="preserve">TartareSauce  </t>
+  </si>
+  <si>
+    <t>[[True, True, True, False, True], [False, False, False, False, False], [False, False, False, False, False]]</t>
+  </si>
+  <si>
+    <t>[[False, True, True, False, False], [False, False, False, False, False], [False, False, False, False, False]]</t>
+  </si>
+  <si>
+    <t>[84.2, 14.44, 14.66]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Only_One_Lap  </t>
+  </si>
+  <si>
+    <t>[[False, False, False, False, False], [False, False, False, False, False], [False, False, False, False, False]]</t>
+  </si>
+  <si>
+    <t>[13.69, 1000.0, 1000.0]</t>
+  </si>
+  <si>
+    <t>slowbutprecise</t>
   </si>
   <si>
     <t>[[True, False, False, False, False], [False, False, False, False, False], [False, False, False, False, False]]</t>
   </si>
   <si>
-    <t>[26.17, 13.2, 13.04]</t>
-  </si>
-  <si>
-    <t>[25.77, 12.44, 12.32]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Only_One_Lap  </t>
-  </si>
-  <si>
-    <t>[[False, False, False, False, False], [False, False, False, False, False], [False, False, False, False, False]]</t>
-  </si>
-  <si>
-    <t>[13.7, 1000.0, 1000.0]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TartareSauce  </t>
-  </si>
-  <si>
-    <t>[[True, True, True, False, False], [True, True, True, False, False], [True, True, True, False, False]]</t>
-  </si>
-  <si>
-    <t>[[False, False, False, False, True], [False, False, False, False, False], [False, False, False, False, False]]</t>
-  </si>
-  <si>
-    <t>[85.83, 14.63, 15.0]</t>
-  </si>
-  <si>
-    <t>[83.16, 11.0, 10.78]</t>
-  </si>
-  <si>
     <t xml:space="preserve">ppff4-1       </t>
   </si>
   <si>
@@ -502,7 +502,7 @@
     <t>[[True, False, True, True, True], [False, False, False, False, False], [False, False, False, False, False]]</t>
   </si>
   <si>
-    <t>[44.7, 1000.0, 1000.0]</t>
+    <t>[44.78, 1000.0, 1000.0]</t>
   </si>
   <si>
     <t xml:space="preserve">Top7_Fave     </t>
@@ -523,9 +523,6 @@
     <t>[39.1, 1.19, 0.86]</t>
   </si>
   <si>
-    <t>slowbutprecise</t>
-  </si>
-  <si>
     <t xml:space="preserve">43RT1K        </t>
   </si>
   <si>
@@ -541,7 +538,7 @@
     <t xml:space="preserve">the_runner    </t>
   </si>
   <si>
-    <t>aerial_rob_fun</t>
+    <t xml:space="preserve">ccka          </t>
   </si>
   <si>
     <t xml:space="preserve">Hey_gringo    </t>
@@ -552,9 +549,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
@@ -589,9 +586,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Aptos Narrow"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -605,8 +609,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Aptos Narrow"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -622,7 +634,21 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -630,45 +656,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Aptos Narrow"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Aptos Narrow"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Aptos Narrow"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Aptos Narrow"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Aptos Narrow"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Aptos Narrow"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -683,14 +671,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Aptos Narrow"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="Aptos Narrow"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -698,6 +679,36 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Aptos Narrow"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -711,27 +722,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Aptos Narrow"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="15"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Aptos Narrow"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Aptos Narrow"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -739,6 +736,18 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -748,7 +757,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -760,13 +787,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -778,25 +859,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -808,31 +889,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -844,49 +907,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -898,31 +919,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -933,6 +930,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -947,6 +959,24 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -966,24 +996,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -995,21 +1007,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1036,148 +1033,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1538,10 +1535,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L42"/>
+  <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="17.25"/>
@@ -1608,7 +1605,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:13">
       <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
@@ -1641,8 +1638,9 @@
       </c>
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="M4" s="5"/>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" s="4" t="s">
         <v>17</v>
       </c>
@@ -1653,7 +1651,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="5">
-        <v>17.27</v>
+        <v>11.68</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>13</v>
@@ -1675,8 +1673,9 @@
       </c>
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="M5" s="5"/>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" s="4" t="s">
         <v>21</v>
       </c>
@@ -1687,7 +1686,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="5">
-        <v>18.85</v>
+        <v>17.27</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>13</v>
@@ -1709,8 +1708,9 @@
       </c>
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="M6" s="5"/>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" s="4" t="s">
         <v>25</v>
       </c>
@@ -1721,7 +1721,7 @@
         <v>5</v>
       </c>
       <c r="D7" s="5">
-        <v>24.5</v>
+        <v>18.85</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>13</v>
@@ -1743,8 +1743,9 @@
       </c>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="M7" s="5"/>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" s="4" t="s">
         <v>29</v>
       </c>
@@ -1752,35 +1753,36 @@
         <v>5</v>
       </c>
       <c r="C8" s="5">
-        <v>4.89</v>
+        <v>5</v>
       </c>
       <c r="D8" s="5">
-        <v>8.69</v>
+        <v>24.5</v>
       </c>
       <c r="E8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="5" t="s">
+      <c r="I8" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="J8" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>33</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="M8" s="5"/>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B9" s="5">
         <v>5</v>
@@ -1789,32 +1791,33 @@
         <v>4.89</v>
       </c>
       <c r="D9" s="5">
-        <v>8.86</v>
+        <v>8.53</v>
       </c>
       <c r="E9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F9" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" s="5" t="s">
+      <c r="I9" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="J9" s="5" t="s">
         <v>37</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>38</v>
       </c>
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="M9" s="5"/>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B10" s="5">
         <v>5</v>
@@ -1823,75 +1826,77 @@
         <v>4.89</v>
       </c>
       <c r="D10" s="5">
-        <v>11.48</v>
+        <v>8.86</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>13</v>
       </c>
       <c r="G10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="I10" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="J10" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>43</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="M10" s="5"/>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B11" s="5">
         <v>5</v>
       </c>
       <c r="C11" s="5">
-        <v>4.78</v>
+        <v>4.89</v>
       </c>
       <c r="D11" s="5">
-        <v>9.31</v>
+        <v>10.84</v>
       </c>
       <c r="E11" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="F11" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H11" s="5" t="s">
+      <c r="I11" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="J11" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>48</v>
       </c>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
-    </row>
-    <row r="12" spans="1:12">
+      <c r="M11" s="5"/>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B12" s="5">
         <v>5</v>
       </c>
       <c r="C12" s="5">
-        <v>4.78</v>
+        <v>4.89</v>
       </c>
       <c r="D12" s="5">
-        <v>11.63</v>
+        <v>11.48</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>13</v>
@@ -1900,23 +1905,24 @@
         <v>13</v>
       </c>
       <c r="G12" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I12" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="J12" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>53</v>
       </c>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
-    </row>
-    <row r="13" spans="1:12">
+      <c r="M12" s="5"/>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B13" s="5">
         <v>5</v>
@@ -1925,32 +1931,33 @@
         <v>4.78</v>
       </c>
       <c r="D13" s="5">
-        <v>12.77</v>
+        <v>9.31</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>13</v>
       </c>
       <c r="G13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="I13" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="J13" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>58</v>
       </c>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
-    </row>
-    <row r="14" spans="1:12">
+      <c r="M13" s="5"/>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B14" s="5">
         <v>5</v>
@@ -1959,591 +1966,608 @@
         <v>4.78</v>
       </c>
       <c r="D14" s="5">
-        <v>12.93</v>
+        <v>10.46</v>
       </c>
       <c r="E14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="I14" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F14" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="H14" s="5" t="s">
+      <c r="J14" s="5" t="s">
         <v>61</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="J14" s="5" t="s">
-        <v>63</v>
       </c>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
-    </row>
-    <row r="15" spans="1:12">
+      <c r="M14" s="5"/>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B15" s="5">
         <v>5</v>
       </c>
       <c r="C15" s="5">
-        <v>4.67</v>
+        <v>4.78</v>
       </c>
       <c r="D15" s="5">
-        <v>10.34</v>
+        <v>12.77</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="F15" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="J15" s="5" t="s">
         <v>65</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="I15" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="J15" s="5" t="s">
-        <v>68</v>
       </c>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
-    </row>
-    <row r="16" spans="1:12">
+      <c r="M15" s="5"/>
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B16" s="5">
         <v>5</v>
       </c>
       <c r="C16" s="5">
-        <v>4.67</v>
+        <v>4.78</v>
       </c>
       <c r="D16" s="5">
-        <v>11.2</v>
+        <v>12.93</v>
       </c>
       <c r="E16" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="J16" s="5" t="s">
         <v>70</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="J16" s="5" t="s">
-        <v>74</v>
       </c>
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
-    </row>
-    <row r="17" spans="1:12">
+      <c r="M16" s="5"/>
+    </row>
+    <row r="17" spans="1:13">
       <c r="A17" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B17" s="5">
         <v>5</v>
       </c>
       <c r="C17" s="5">
-        <v>4.22</v>
+        <v>4.67</v>
       </c>
       <c r="D17" s="5">
-        <v>19.64</v>
+        <v>10.34</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>55</v>
+        <v>13</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
-    </row>
-    <row r="18" spans="1:12">
+      <c r="M17" s="5"/>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18" s="4" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B18" s="5">
         <v>5</v>
       </c>
       <c r="C18" s="5">
-        <v>3.33</v>
+        <v>4.67</v>
       </c>
       <c r="D18" s="5">
-        <v>511.07</v>
+        <v>11.2</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
-    </row>
-    <row r="19" spans="1:12">
+      <c r="M18" s="5"/>
+    </row>
+    <row r="19" spans="1:13">
       <c r="A19" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B19" s="5">
+        <v>5</v>
+      </c>
+      <c r="C19" s="5">
+        <v>4.67</v>
+      </c>
+      <c r="D19" s="5">
+        <v>11.94</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="J19" s="5" t="s">
         <v>86</v>
-      </c>
-      <c r="B19" s="5">
-        <v>4.67</v>
-      </c>
-      <c r="C19" s="5">
-        <v>4.89</v>
-      </c>
-      <c r="D19" s="5">
-        <v>11.25</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="J19" s="5" t="s">
-        <v>90</v>
       </c>
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
-    </row>
-    <row r="20" spans="1:12">
+      <c r="M19" s="5"/>
+    </row>
+    <row r="20" spans="1:13">
       <c r="A20" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B20" s="5">
+        <v>5</v>
+      </c>
+      <c r="C20" s="5">
+        <v>4.56</v>
+      </c>
+      <c r="D20" s="5">
+        <v>8.4</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="J20" s="5" t="s">
         <v>91</v>
-      </c>
-      <c r="B20" s="5">
-        <v>4.67</v>
-      </c>
-      <c r="C20" s="5">
-        <v>4.67</v>
-      </c>
-      <c r="D20" s="5">
-        <v>19.56</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="I20" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="J20" s="5" t="s">
-        <v>95</v>
       </c>
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
-    </row>
-    <row r="21" spans="1:12">
+      <c r="M20" s="5"/>
+    </row>
+    <row r="21" spans="1:13">
       <c r="A21" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B21" s="5">
+        <v>5</v>
+      </c>
+      <c r="C21" s="5">
+        <v>4.22</v>
+      </c>
+      <c r="D21" s="5">
+        <v>19.64</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="I21" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B21" s="5">
-        <v>4.67</v>
-      </c>
-      <c r="C21" s="5">
-        <v>3.78</v>
-      </c>
-      <c r="D21" s="5">
-        <v>11.19</v>
-      </c>
-      <c r="E21" s="5" t="s">
+      <c r="J21" s="5" t="s">
         <v>97</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="I21" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="J21" s="5" t="s">
-        <v>102</v>
       </c>
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
-    </row>
-    <row r="22" spans="1:12">
+      <c r="M21" s="5"/>
+    </row>
+    <row r="22" spans="1:13">
       <c r="A22" s="4" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B22" s="5">
-        <v>4.67</v>
+        <v>5</v>
       </c>
       <c r="C22" s="5">
-        <v>3.78</v>
+        <v>3.33</v>
       </c>
       <c r="D22" s="5">
-        <v>340.39</v>
+        <v>511.07</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>13</v>
+        <v>99</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>13</v>
+        <v>99</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
-    </row>
-    <row r="23" spans="1:12">
+      <c r="M22" s="5"/>
+    </row>
+    <row r="23" spans="1:13">
       <c r="A23" s="4" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B23" s="5">
         <v>4.67</v>
       </c>
       <c r="C23" s="5">
-        <v>3</v>
+        <v>4.89</v>
       </c>
       <c r="D23" s="5">
-        <v>348.28</v>
+        <v>11.25</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>109</v>
+        <v>13</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>111</v>
+        <v>13</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="J23" s="5" t="s">
         <v>107</v>
       </c>
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
-    </row>
-    <row r="24" spans="1:12">
+      <c r="M23" s="5"/>
+    </row>
+    <row r="24" spans="1:13">
       <c r="A24" s="4" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B24" s="5">
-        <v>4.33</v>
+        <v>4.67</v>
       </c>
       <c r="C24" s="5">
-        <v>4.44</v>
+        <v>4.67</v>
       </c>
       <c r="D24" s="5">
-        <v>10.86</v>
+        <v>19.56</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>13</v>
+        <v>109</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>13</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>115</v>
+        <v>13</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
-    </row>
-    <row r="25" spans="1:12">
+      <c r="M24" s="5"/>
+    </row>
+    <row r="25" spans="1:13">
       <c r="A25" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B25" s="5">
+        <v>4.67</v>
+      </c>
+      <c r="C25" s="5">
+        <v>3.78</v>
+      </c>
+      <c r="D25" s="5">
+        <v>11.19</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="J25" s="5" t="s">
         <v>119</v>
-      </c>
-      <c r="B25" s="5">
-        <v>4.33</v>
-      </c>
-      <c r="C25" s="5">
-        <v>4.22</v>
-      </c>
-      <c r="D25" s="5">
-        <v>15.41</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H25" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="I25" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="J25" s="5" t="s">
-        <v>124</v>
       </c>
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
-    </row>
-    <row r="26" spans="1:12">
+      <c r="M25" s="5"/>
+    </row>
+    <row r="26" spans="1:13">
       <c r="A26" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B26" s="5">
+        <v>4.67</v>
+      </c>
+      <c r="C26" s="5">
+        <v>3</v>
+      </c>
+      <c r="D26" s="5">
+        <v>348.28</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="I26" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="B26" s="5">
-        <v>4.33</v>
-      </c>
-      <c r="C26" s="5">
-        <v>3.67</v>
-      </c>
-      <c r="D26" s="5">
-        <v>9.77</v>
-      </c>
-      <c r="E26" s="5" t="s">
+      <c r="J26" s="5" t="s">
         <v>126</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H26" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="I26" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="J26" s="5" t="s">
-        <v>129</v>
       </c>
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
-    </row>
-    <row r="27" spans="1:12">
+      <c r="M26" s="5"/>
+    </row>
+    <row r="27" spans="1:13">
       <c r="A27" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B27" s="5">
         <v>4.33</v>
       </c>
       <c r="C27" s="5">
-        <v>3.22</v>
+        <v>4.22</v>
       </c>
       <c r="D27" s="5">
-        <v>339.19</v>
+        <v>15.41</v>
       </c>
       <c r="E27" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="I27" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="F27" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="H27" s="5" t="s">
+      <c r="J27" s="5" t="s">
         <v>132</v>
-      </c>
-      <c r="I27" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="J27" s="5" t="s">
-        <v>107</v>
       </c>
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
-    </row>
-    <row r="28" spans="1:12">
+      <c r="M27" s="5"/>
+    </row>
+    <row r="28" spans="1:13">
       <c r="A28" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B28" s="5">
         <v>4.33</v>
       </c>
       <c r="C28" s="5">
-        <v>2.67</v>
+        <v>3.67</v>
       </c>
       <c r="D28" s="5">
-        <v>508</v>
+        <v>9.77</v>
       </c>
       <c r="E28" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H28" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="I28" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="G28" s="5" t="s">
+      <c r="J28" s="5" t="s">
         <v>137</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="I28" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="J28" s="5" t="s">
-        <v>140</v>
       </c>
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
-    </row>
-    <row r="29" spans="1:12">
+      <c r="M28" s="5"/>
+    </row>
+    <row r="29" spans="1:13">
       <c r="A29" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B29" s="5">
+        <v>4.33</v>
+      </c>
+      <c r="C29" s="5">
+        <v>2.67</v>
+      </c>
+      <c r="D29" s="5">
+        <v>508</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="G29" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="B29" s="5">
-        <v>4</v>
-      </c>
-      <c r="C29" s="5">
-        <v>4</v>
-      </c>
-      <c r="D29" s="5">
-        <v>13.34</v>
-      </c>
-      <c r="E29" s="5" t="s">
+      <c r="H29" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="F29" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="G29" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="H29" s="5" t="s">
+      <c r="I29" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="I29" s="5" t="s">
+      <c r="J29" s="5" t="s">
         <v>144</v>
-      </c>
-      <c r="J29" s="5" t="s">
-        <v>145</v>
       </c>
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
-    </row>
-    <row r="30" spans="1:12">
+      <c r="M29" s="5"/>
+    </row>
+    <row r="30" spans="1:13">
       <c r="A30" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B30" s="5">
+        <v>4</v>
+      </c>
+      <c r="C30" s="5">
+        <v>4</v>
+      </c>
+      <c r="D30" s="5">
+        <v>13.34</v>
+      </c>
+      <c r="E30" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="B30" s="5">
-        <v>3.67</v>
-      </c>
-      <c r="C30" s="5">
-        <v>2.89</v>
-      </c>
-      <c r="D30" s="5">
-        <v>341.83</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="F30" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="H30" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="G30" s="5" t="s">
+      <c r="I30" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="H30" s="5" t="s">
+      <c r="J30" s="5" t="s">
         <v>149</v>
-      </c>
-      <c r="I30" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="J30" s="5" t="s">
-        <v>107</v>
       </c>
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
-    </row>
-    <row r="31" spans="1:12">
+      <c r="M30" s="5"/>
+    </row>
+    <row r="31" spans="1:13">
       <c r="A31" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B31" s="5">
+        <v>3.67</v>
+      </c>
+      <c r="C31" s="5">
+        <v>2.33</v>
+      </c>
+      <c r="D31" s="5">
+        <v>671.52</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F31" s="5" t="s">
         <v>151</v>
-      </c>
-      <c r="B31" s="5">
-        <v>3.33</v>
-      </c>
-      <c r="C31" s="5">
-        <v>1.11</v>
-      </c>
-      <c r="D31" s="5">
-        <v>1000</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>111</v>
       </c>
       <c r="G31" s="5" t="s">
         <v>152</v>
@@ -2552,153 +2576,158 @@
         <v>153</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="K31" s="5"/>
       <c r="L31" s="5"/>
-    </row>
-    <row r="32" spans="1:12">
+      <c r="M31" s="5"/>
+    </row>
+    <row r="32" spans="1:13">
       <c r="A32" s="4" t="s">
         <v>154</v>
       </c>
       <c r="B32" s="5">
-        <v>3</v>
+        <v>3.33</v>
       </c>
       <c r="C32" s="5">
-        <v>2.78</v>
+        <v>1.11</v>
       </c>
       <c r="D32" s="5">
-        <v>341.9</v>
+        <v>1000</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>13</v>
+        <v>123</v>
       </c>
       <c r="F32" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G32" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="G32" s="5" t="s">
+      <c r="H32" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="H32" s="5" t="s">
-        <v>157</v>
-      </c>
       <c r="I32" s="5" t="s">
-        <v>158</v>
+        <v>126</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
-    </row>
-    <row r="33" spans="1:12">
+      <c r="M32" s="5"/>
+    </row>
+    <row r="33" spans="1:13">
       <c r="A33" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B33" s="5">
-        <v>2.33</v>
+        <v>3</v>
       </c>
       <c r="C33" s="5">
-        <v>0.78</v>
+        <v>1</v>
       </c>
       <c r="D33" s="5">
         <v>1000</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>152</v>
+        <v>123</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>160</v>
+        <v>134</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>162</v>
+        <v>126</v>
       </c>
       <c r="K33" s="5"/>
       <c r="L33" s="5"/>
-    </row>
-    <row r="34" spans="1:12">
+      <c r="M33" s="5"/>
+    </row>
+    <row r="34" spans="1:13">
       <c r="A34" s="4" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B34" s="5">
-        <v>2</v>
+        <v>2.33</v>
       </c>
       <c r="C34" s="5">
-        <v>1.11</v>
+        <v>0.78</v>
       </c>
       <c r="D34" s="5">
-        <v>12.26</v>
+        <v>1000</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>166</v>
+        <v>126</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>167</v>
+        <v>126</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="K34" s="5"/>
       <c r="L34" s="5"/>
-    </row>
-    <row r="35" spans="1:12">
+      <c r="M34" s="5"/>
+    </row>
+    <row r="35" spans="1:13">
       <c r="A35" s="4" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="B35" s="5">
         <v>2</v>
       </c>
       <c r="C35" s="5">
-        <v>0.67</v>
+        <v>1.11</v>
       </c>
       <c r="D35" s="5">
-        <v>1000</v>
+        <v>12.26</v>
       </c>
       <c r="E35" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="F35" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="F35" s="5" t="s">
-        <v>126</v>
-      </c>
       <c r="G35" s="5" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>107</v>
+        <v>166</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>107</v>
+        <v>167</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>107</v>
+        <v>168</v>
       </c>
       <c r="K35" s="5"/>
       <c r="L35" s="5"/>
-    </row>
-    <row r="36" spans="1:12">
+      <c r="M35" s="5"/>
+    </row>
+    <row r="36" spans="1:13">
       <c r="A36" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B36" s="5">
         <v>0</v>
@@ -2710,29 +2739,30 @@
         <v>1000</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="K36" s="5"/>
       <c r="L36" s="5"/>
-    </row>
-    <row r="37" spans="1:12">
+      <c r="M36" s="5"/>
+    </row>
+    <row r="37" spans="1:13">
       <c r="A37" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B37" s="5">
         <v>0</v>
@@ -2744,29 +2774,30 @@
         <v>1000</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="I37" s="5" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="K37" s="5"/>
       <c r="L37" s="5"/>
-    </row>
-    <row r="38" spans="1:12">
+      <c r="M37" s="5"/>
+    </row>
+    <row r="38" spans="1:13">
       <c r="A38" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B38" s="5">
         <v>0</v>
@@ -2778,29 +2809,30 @@
         <v>1000</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="I38" s="5" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="K38" s="5"/>
       <c r="L38" s="5"/>
-    </row>
-    <row r="39" spans="1:12">
+      <c r="M38" s="5"/>
+    </row>
+    <row r="39" spans="1:13">
       <c r="A39" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B39" s="5">
         <v>0</v>
@@ -2812,29 +2844,30 @@
         <v>1000</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="I39" s="5" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="K39" s="5"/>
       <c r="L39" s="5"/>
-    </row>
-    <row r="40" spans="1:12">
+      <c r="M39" s="5"/>
+    </row>
+    <row r="40" spans="1:13">
       <c r="A40" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B40" s="5">
         <v>0</v>
@@ -2846,29 +2879,30 @@
         <v>1000</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="K40" s="5"/>
       <c r="L40" s="5"/>
-    </row>
-    <row r="41" spans="1:12">
+      <c r="M40" s="5"/>
+    </row>
+    <row r="41" spans="1:13">
       <c r="A41" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B41" s="5">
         <v>0</v>
@@ -2880,29 +2914,30 @@
         <v>1000</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="I41" s="5" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="K41" s="5"/>
       <c r="L41" s="5"/>
-    </row>
-    <row r="42" spans="1:12">
+      <c r="M41" s="5"/>
+    </row>
+    <row r="42" spans="1:13">
       <c r="A42" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B42" s="5">
         <v>0</v>
@@ -2914,25 +2949,71 @@
         <v>1000</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="I42" s="5" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="K42" s="5"/>
       <c r="L42" s="5"/>
+      <c r="M42" s="5"/>
+    </row>
+    <row r="43" spans="1:13">
+      <c r="A43" s="5"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
+      <c r="I43" s="5"/>
+      <c r="J43" s="5"/>
+      <c r="K43" s="5"/>
+      <c r="L43" s="5"/>
+      <c r="M43" s="5"/>
+    </row>
+    <row r="44" spans="1:13">
+      <c r="A44" s="5"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
+      <c r="I44" s="5"/>
+      <c r="J44" s="5"/>
+      <c r="K44" s="5"/>
+      <c r="L44" s="5"/>
+      <c r="M44" s="5"/>
+    </row>
+    <row r="45" spans="1:13">
+      <c r="A45" s="5"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="5"/>
+      <c r="J45" s="5"/>
+      <c r="K45" s="5"/>
+      <c r="L45" s="5"/>
+      <c r="M45" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
Update grading_full to only show the best result (most recent results on moodle)
</commit_message>
<xml_diff>
--- a/docs/assignment/grading_full.xlsx
+++ b/docs/assignment/grading_full.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="314">
   <si>
     <t>Grading Data</t>
   </si>
@@ -70,25 +70,25 @@
     <t xml:space="preserve">crasyJ        </t>
   </si>
   <si>
-    <t>[59.15, 11.81, 10.48]</t>
-  </si>
-  <si>
-    <t>[72.11, 11.75, 11.18]</t>
-  </si>
-  <si>
-    <t>[42.76, 10.31, 9.27]</t>
+    <t>[66.92, 11.86, 10.88]</t>
+  </si>
+  <si>
+    <t>[80.47, 10.72, 10.07]</t>
+  </si>
+  <si>
+    <t>[66.98, 10.56, 9.02]</t>
   </si>
   <si>
     <t xml:space="preserve">CPT           </t>
   </si>
   <si>
-    <t>[93.1, 11.84, 11.72]</t>
-  </si>
-  <si>
-    <t>[80.82, 11.13, 11.06]</t>
-  </si>
-  <si>
-    <t>[68.37, 10.23, 9.86]</t>
+    <t>[85.54, 11.79, 11.66]</t>
+  </si>
+  <si>
+    <t>[85.7, 11.11, 11.02]</t>
+  </si>
+  <si>
+    <t>[85.59, 10.22, 9.84]</t>
   </si>
   <si>
     <t xml:space="preserve">avocado       </t>
@@ -103,6 +103,18 @@
     <t>[68.58, 11.78, 10.18]</t>
   </si>
   <si>
+    <t xml:space="preserve">Albatros      </t>
+  </si>
+  <si>
+    <t>[113.54, 12.49, 12.26]</t>
+  </si>
+  <si>
+    <t>[122.03, 11.68, 11.67]</t>
+  </si>
+  <si>
+    <t>[89.78, 10.65, 10.58]</t>
+  </si>
+  <si>
     <t xml:space="preserve">LuraIL        </t>
   </si>
   <si>
@@ -187,16 +199,28 @@
     <t>[16.46, 16.09, 17.68]</t>
   </si>
   <si>
+    <t xml:space="preserve">Malkarenn     </t>
+  </si>
+  <si>
+    <t>[34.01, 17.91, 17.59]</t>
+  </si>
+  <si>
+    <t>[33.54, 17.1, 17.19]</t>
+  </si>
+  <si>
+    <t>[33.44, 17.1, 16.75]</t>
+  </si>
+  <si>
     <t xml:space="preserve">snail         </t>
   </si>
   <si>
-    <t>[79.06, 18.33, 18.26]</t>
-  </si>
-  <si>
-    <t>[74.62, 18.26, 18.34]</t>
-  </si>
-  <si>
-    <t>[70.49, 17.28, 16.91]</t>
+    <t>[77.5, 18.35, 18.22]</t>
+  </si>
+  <si>
+    <t>[73.97, 18.21, 18.1]</t>
+  </si>
+  <si>
+    <t>[71.72, 17.22, 17.04]</t>
   </si>
   <si>
     <t xml:space="preserve">AGN_v1        </t>
@@ -223,6 +247,18 @@
     <t>[52.6, 23.36, 24.09]</t>
   </si>
   <si>
+    <t xml:space="preserve">USAIN_BOLD    </t>
+  </si>
+  <si>
+    <t>[70.92, 29.25, 23.14]</t>
+  </si>
+  <si>
+    <t>[62.62, 25.42, 21.9]</t>
+  </si>
+  <si>
+    <t>[59.79, 25.98, 21.3]</t>
+  </si>
+  <si>
     <t xml:space="preserve">Katrix        </t>
   </si>
   <si>
@@ -235,19 +271,61 @@
     <t>[81.52, 44.61, 36.45]</t>
   </si>
   <si>
-    <t xml:space="preserve">Albatros      </t>
+    <t>JojoDeCrissier</t>
+  </si>
+  <si>
+    <t>[[True, True, True, True, True], [True, True, True, True, True], [False, True, True, True, True]]</t>
+  </si>
+  <si>
+    <t>[67.98, 9.33, 9.32]</t>
+  </si>
+  <si>
+    <t>[105.38, 8.35, 8.36]</t>
+  </si>
+  <si>
+    <t>[56.62, 7.9, 7.89]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pizza         </t>
+  </si>
+  <si>
+    <t>[[True, True, True, True, True], [True, True, True, True, True], [True, False, True, True, True]]</t>
+  </si>
+  <si>
+    <t>[55.02, 9.65, 9.58]</t>
+  </si>
+  <si>
+    <t>[81.87, 9.25, 9.26]</t>
+  </si>
+  <si>
+    <t>[64.02, 7.78, 7.66]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tau           </t>
   </si>
   <si>
     <t>[[True, True, True, True, True], [True, False, True, True, True], [True, True, True, True, True]]</t>
   </si>
   <si>
-    <t>[113.87, 11.63, 11.44]</t>
-  </si>
-  <si>
-    <t>[109.41, 10.85, 10.86]</t>
-  </si>
-  <si>
-    <t>[92.18, 9.87, 9.8]</t>
+    <t>[44.54, 10.94, 10.93]</t>
+  </si>
+  <si>
+    <t>[44.46, 10.85, 10.85]</t>
+  </si>
+  <si>
+    <t>[47.29, 10.74, 10.76]</t>
+  </si>
+  <si>
+    <t>my_assignment.</t>
+  </si>
+  <si>
+    <t>[47.27, 11.98, 11.79]</t>
+  </si>
+  <si>
+    <t>[51.58, 11.26, 11.1]</t>
+  </si>
+  <si>
+    <t>[40.65, 11.02, 11.18]</t>
   </si>
   <si>
     <t>pigeon_mal_nou</t>
@@ -295,64 +373,85 @@
     <t>[83.93, 10.54, 10.72]</t>
   </si>
   <si>
-    <t>JojoDeCrissier</t>
-  </si>
-  <si>
-    <t>[[True, True, True, True, True], [True, True, True, True, True], [False, True, True, True, True]]</t>
-  </si>
-  <si>
-    <t>[98.64, 11.58, 11.64]</t>
-  </si>
-  <si>
-    <t>[95.69, 11.16, 10.97]</t>
-  </si>
-  <si>
-    <t>[83.5, 9.9, 10.05]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Malkarenn     </t>
+    <t xml:space="preserve">ratatouille   </t>
+  </si>
+  <si>
+    <t>[[True, True, True, True, True], [True, True, True, False, True], [True, True, True, False, True]]</t>
+  </si>
+  <si>
+    <t>[91.5, 13.29, 12.67]</t>
+  </si>
+  <si>
+    <t>[130.19, 12.6, 11.89]</t>
+  </si>
+  <si>
+    <t>[119.86, 11.37, 10.79]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adv_v3        </t>
+  </si>
+  <si>
+    <t>[[True, True, True, True, True], [True, True, True, True, False], [True, True, True, True, True]]</t>
+  </si>
+  <si>
+    <t>[63.03, 13.5, 13.58]</t>
+  </si>
+  <si>
+    <t>[75.49, 13.33, 13.06]</t>
+  </si>
+  <si>
+    <t>[50.19, 12.19, 11.9]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gg_2          </t>
+  </si>
+  <si>
+    <t>[[True, True, True, True, True], [False, True, True, True, True], [True, True, True, True, True]]</t>
+  </si>
+  <si>
+    <t>[[True, True, True, True, True], [True, True, True, True, True], [True, True, True, True, False]]</t>
+  </si>
+  <si>
+    <t>[[True, True, True, True, True], [True, True, True, True, True], [True, True, False, True, True]]</t>
+  </si>
+  <si>
+    <t>[76.2, 11.62, 11.59]</t>
+  </si>
+  <si>
+    <t>[70.74, 11.32, 11.28]</t>
+  </si>
+  <si>
+    <t>[72.82, 10.66, 10.75]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">odermatt      </t>
+  </si>
+  <si>
+    <t>[[True, True, True, True, True], [True, True, False, True, True], [True, True, False, True, False]]</t>
+  </si>
+  <si>
+    <t>[25.87, 12.49, 12.41]</t>
+  </si>
+  <si>
+    <t>[24.13, 11.85, 11.73]</t>
+  </si>
+  <si>
+    <t>[23.9, 11.37, 11.78]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mmm128        </t>
   </si>
   <si>
     <t>[[True, True, True, True, True], [True, True, False, True, True], [True, True, False, True, True]]</t>
   </si>
   <si>
-    <t>[36.14, 11.82, 10.99]</t>
-  </si>
-  <si>
-    <t>[37.95, 12.32, 11.3]</t>
-  </si>
-  <si>
-    <t>[30.9, 11.14, 8.99]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ratatouille   </t>
-  </si>
-  <si>
-    <t>[[True, True, True, True, True], [True, True, True, False, True], [True, True, True, False, True]]</t>
-  </si>
-  <si>
-    <t>[91.5, 13.29, 12.67]</t>
-  </si>
-  <si>
-    <t>[130.19, 12.6, 11.89]</t>
-  </si>
-  <si>
-    <t>[119.86, 11.37, 10.79]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USAIN_BOLD    </t>
-  </si>
-  <si>
-    <t>[[True, True, True, True, True], [True, False, True, True, True], [True, True, False, True, True]]</t>
-  </si>
-  <si>
-    <t>[81.09, 32.63, 25.18]</t>
-  </si>
-  <si>
-    <t>[63.05, 26.5, 22.76]</t>
-  </si>
-  <si>
-    <t>[61.21, 26.74, 21.28]</t>
+    <t>[46.62, 15.8, 15.32]</t>
+  </si>
+  <si>
+    <t>[54.17, 15.21, 15.09]</t>
+  </si>
+  <si>
+    <t>[46.32, 15.38, 15.38]</t>
   </si>
   <si>
     <t>Easyyy_Submiss</t>
@@ -370,61 +469,55 @@
     <t>[59.44, 15.87, 15.99]</t>
   </si>
   <si>
-    <t xml:space="preserve">gg_2          </t>
-  </si>
-  <si>
-    <t>[[True, True, True, True, True], [False, True, True, True, True], [True, True, True, True, True]]</t>
-  </si>
-  <si>
-    <t>[[True, True, True, True, True], [True, True, False, True, True], [True, True, True, True, True]]</t>
-  </si>
-  <si>
-    <t>[74.12, 11.56, 11.38]</t>
-  </si>
-  <si>
-    <t>[94.75, 11.06, 11.2]</t>
-  </si>
-  <si>
-    <t>[76.09, 10.86, 10.58]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pizza         </t>
+    <t xml:space="preserve">ccka_         </t>
+  </si>
+  <si>
+    <t>[[True, True, True, True, True], [True, True, True, True, False], [False, False, True, True, False]]</t>
+  </si>
+  <si>
+    <t>[[True, True, True, True, True], [True, True, True, False, False], [True, True, True, False, False]]</t>
+  </si>
+  <si>
+    <t>[59.36, 10.41, 9.41]</t>
+  </si>
+  <si>
+    <t>[58.82, 10.18, 9.22]</t>
+  </si>
+  <si>
+    <t>[52.23, 10.02, 9.22]</t>
+  </si>
+  <si>
+    <t>kazf_submissio</t>
   </si>
   <si>
     <t>[[True, True, True, True, True], [False, False, False, False, False], [False, False, False, False, False]]</t>
   </si>
   <si>
-    <t>[55.46, 9.72, 9.36]</t>
+    <t>[24.4, 1000.0, 1000.0]</t>
+  </si>
+  <si>
+    <t>[23.55, 17.87, 17.36]</t>
+  </si>
+  <si>
+    <t>[22.14, 14.65, 14.62]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CrazyBoy      </t>
+  </si>
+  <si>
+    <t>[[True, True, True, True, True], [False, False, False, True, True], [True, True, True, True, True]]</t>
+  </si>
+  <si>
+    <t>[[True, True, True, True, True], [True, True, True, True, False], [True, True, True, True, False]]</t>
+  </si>
+  <si>
+    <t>[114.14, 11.67, 10.81]</t>
   </si>
   <si>
     <t>[1000.0, 1000.0, 1000.0]</t>
   </si>
   <si>
-    <t>[79.06, 7.83, 7.73]</t>
-  </si>
-  <si>
-    <t>kazf_submissio</t>
-  </si>
-  <si>
-    <t>[24.4, 1000.0, 1000.0]</t>
-  </si>
-  <si>
-    <t>[23.55, 17.87, 17.36]</t>
-  </si>
-  <si>
-    <t>[22.14, 14.65, 14.62]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">adv_v3        </t>
-  </si>
-  <si>
-    <t>[[True, True, True, True, True], [True, True, True, True, False], [True, True, True, True, True]]</t>
-  </si>
-  <si>
-    <t>[75.82, 14.16, 14.1]</t>
-  </si>
-  <si>
-    <t>[49.57, 12.3, 11.92]</t>
+    <t>[117.07, 9.01, 8.83]</t>
   </si>
   <si>
     <t xml:space="preserve">ppf4-2        </t>
@@ -490,6 +583,27 @@
     <t>[20.73, 19.13, 14.71]</t>
   </si>
   <si>
+    <t xml:space="preserve">Ammann        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">rendu0        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AerialEM3     </t>
+  </si>
+  <si>
+    <t>[[True, True, False, True, True], [True, True, True, True, True], [True, True, True, True, True]]</t>
+  </si>
+  <si>
+    <t>[32.26, 11.69, 11.58]</t>
+  </si>
+  <si>
+    <t>[32.95, 11.16, 11.14]</t>
+  </si>
+  <si>
+    <t>[32.8, 10.69, 10.78]</t>
+  </si>
+  <si>
     <t xml:space="preserve">iLoveSat      </t>
   </si>
   <si>
@@ -520,30 +634,12 @@
     <t>[39.76, 12.3, 10.52]</t>
   </si>
   <si>
-    <t xml:space="preserve">mmm128        </t>
-  </si>
-  <si>
-    <t>[[True, False, True, True, True], [True, False, True, True, True], [True, False, True, True, True]]</t>
-  </si>
-  <si>
-    <t>[82.42, 24.38, 23.57]</t>
-  </si>
-  <si>
-    <t>[80.48, 23.26, 23.04]</t>
-  </si>
-  <si>
-    <t>[83.6, 24.27, 23.96]</t>
-  </si>
-  <si>
     <t xml:space="preserve">Hey_gringo    </t>
   </si>
   <si>
     <t>[[True, False, True, True, True], [True, True, True, True, False], [True, True, True, True, True]]</t>
   </si>
   <si>
-    <t>[[True, True, True, True, True], [True, True, True, True, True], [True, True, True, True, False]]</t>
-  </si>
-  <si>
     <t>[68.06, 12.38, 13.02]</t>
   </si>
   <si>
@@ -553,27 +649,12 @@
     <t>[72.68, 11.24, 11.76]</t>
   </si>
   <si>
-    <t xml:space="preserve">ccka_         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ammann        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">rendu0        </t>
-  </si>
-  <si>
     <t>fastandfurious</t>
   </si>
   <si>
     <t>[[True, False, True, True, True], [False, False, True, True, False], [False, False, True, True, False]]</t>
   </si>
   <si>
-    <t>[[True, True, True, True, True], [True, True, True, True, True], [True, False, True, True, True]]</t>
-  </si>
-  <si>
-    <t>[[True, True, True, True, True], [True, True, True, True, False], [True, True, True, True, False]]</t>
-  </si>
-  <si>
     <t>[73.37, 16.0, 15.94]</t>
   </si>
   <si>
@@ -610,21 +691,6 @@
     <t>[44.13, 13.38, 12.96]</t>
   </si>
   <si>
-    <t xml:space="preserve">AerialEM3     </t>
-  </si>
-  <si>
-    <t>[[True, True, False, True, False], [True, True, False, True, False], [True, True, False, True, False]]</t>
-  </si>
-  <si>
-    <t>[32.14, 11.94, 11.85]</t>
-  </si>
-  <si>
-    <t>[29.7, 9.87, 9.9]</t>
-  </si>
-  <si>
-    <t>[33.06, 10.71, 10.7]</t>
-  </si>
-  <si>
     <t>bulldozer_on_w</t>
   </si>
   <si>
@@ -667,27 +733,75 @@
     <t>[77.5, 11.68, 11.6]</t>
   </si>
   <si>
+    <t>MatheoTailland</t>
+  </si>
+  <si>
+    <t>[[True, True, True, False, False], [False, False, False, False, False], [False, False, False, False, False]]</t>
+  </si>
+  <si>
+    <t>[43.72, 14.08, 13.58]</t>
+  </si>
+  <si>
+    <t>[33.99, 14.53, 13.99]</t>
+  </si>
+  <si>
     <t xml:space="preserve">Joko          </t>
   </si>
   <si>
-    <t>[[True, True, True, False, False], [False, False, False, False, False], [False, False, False, False, False]]</t>
-  </si>
-  <si>
     <t>[28.1, 18.47, 18.06]</t>
   </si>
   <si>
     <t>[41.88, 16.91, 17.33]</t>
   </si>
   <si>
+    <t xml:space="preserve">Top7_Fave     </t>
+  </si>
+  <si>
+    <t>[[True, True, True, True, False], [True, False, False, False, False], [False, False, False, False, False]]</t>
+  </si>
+  <si>
+    <t>[[True, False, True, True, True], [True, False, False, True, True], [False, False, False, True, True]]</t>
+  </si>
+  <si>
+    <t>[[True, True, True, True, True], [True, False, True, True, False], [True, False, True, True, False]]</t>
+  </si>
+  <si>
+    <t>[35.26, 22.96, 22.79]</t>
+  </si>
+  <si>
+    <t>[26.73, 21.82, 21.86]</t>
+  </si>
+  <si>
+    <t>[27.17, 20.98, 21.32]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">slowking      </t>
+  </si>
+  <si>
+    <t>[[True, True, True, True, True], [True, True, False, True, False], [True, True, True, True, False]]</t>
+  </si>
+  <si>
+    <t>[[True, True, False, True, True], [False, False, False, False, False], [False, False, False, False, False]]</t>
+  </si>
+  <si>
+    <t>[[True, True, True, True, False], [True, True, False, True, True], [False, False, False, False, False]]</t>
+  </si>
+  <si>
+    <t>[20.19, 15.41, 15.23]</t>
+  </si>
+  <si>
+    <t>[23.0, 1000.0, 1000.0]</t>
+  </si>
+  <si>
+    <t>[52.65, 17.38, 1000.0]</t>
+  </si>
+  <si>
     <t xml:space="preserve">43RT1K        </t>
   </si>
   <si>
     <t>[[True, True, True, True, True], [True, True, True, True, True], [False, False, False, False, False]]</t>
   </si>
   <si>
-    <t>[[True, True, False, True, True], [False, False, False, False, False], [False, False, False, False, False]]</t>
-  </si>
-  <si>
     <t>[[True, False, True, True, True], [True, False, True, True, True], [False, False, False, False, False]]</t>
   </si>
   <si>
@@ -697,111 +811,72 @@
     <t>[19.32, 10.1, 1000.0]</t>
   </si>
   <si>
-    <t>MatheoTailland</t>
-  </si>
-  <si>
-    <t>[[True, True, True, False, True], [True, True, True, False, True], [True, False, True, False, True]]</t>
-  </si>
-  <si>
-    <t>[[True, False, True, False, True], [True, True, True, False, True], [True, True, True, False, True]]</t>
-  </si>
-  <si>
-    <t>[43.12, 15.53, 14.66]</t>
-  </si>
-  <si>
-    <t>[31.3, 13.42, 13.91]</t>
-  </si>
-  <si>
-    <t>[42.57, 15.83, 14.78]</t>
+    <t xml:space="preserve">DODO_V1       </t>
+  </si>
+  <si>
+    <t>[[True, True, True, True, False], [False, False, False, False, False], [False, False, False, False, False]]</t>
+  </si>
+  <si>
+    <t>[30.05, 1000.0, 1000.0]</t>
+  </si>
+  <si>
+    <t>[26.78, 1000.0, 1000.0]</t>
   </si>
   <si>
     <t xml:space="preserve">MaydayMayday2 </t>
   </si>
   <si>
-    <t>[71.43, 14.83, 15.03]</t>
-  </si>
-  <si>
-    <t>[75.66, 13.8, 13.73]</t>
-  </si>
-  <si>
-    <t>[81.73, 12.68, 12.71]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DODO_V1       </t>
-  </si>
-  <si>
-    <t>[[True, True, True, True, False], [False, False, False, False, False], [False, False, False, False, False]]</t>
-  </si>
-  <si>
-    <t>[30.05, 1000.0, 1000.0]</t>
-  </si>
-  <si>
-    <t>[26.78, 1000.0, 1000.0]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tau           </t>
+    <t>[[False, True, True, True, True], [False, True, True, True, True], [False, True, True, True, True]]</t>
+  </si>
+  <si>
+    <t>[68.03, 13.56, 13.65]</t>
+  </si>
+  <si>
+    <t>[73.78, 13.85, 13.69]</t>
+  </si>
+  <si>
+    <t>[86.1, 12.69, 12.62]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zooooooom     </t>
+  </si>
+  <si>
+    <t>[[True, True, True, True, True], [False, False, False, False, False], [False, False, False, True, True]]</t>
+  </si>
+  <si>
+    <t>[[True, True, False, True, False], [False, True, True, True, False], [False, True, True, True, False]]</t>
+  </si>
+  <si>
+    <t>[[True, False, True, True, True], [False, False, True, True, False], [False, False, False, True, False]]</t>
+  </si>
+  <si>
+    <t>[24.77, 8.8, 9.7]</t>
+  </si>
+  <si>
+    <t>[25.27, 9.49, 10.03]</t>
+  </si>
+  <si>
+    <t>[32.08, 9.67, 9.66]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DUPLO_DRONUS  </t>
+  </si>
+  <si>
+    <t>[60.17, 12.1, 12.06]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kambunji      </t>
   </si>
   <si>
     <t>[[True, True, False, False, False], [False, False, False, False, False], [False, False, False, False, False]]</t>
   </si>
   <si>
-    <t>[46.94, 10.94, 10.92]</t>
-  </si>
-  <si>
-    <t>[46.06, 10.85, 10.86]</t>
-  </si>
-  <si>
-    <t>my_assignment.</t>
-  </si>
-  <si>
-    <t>[[True, True, True, True, True], [True, True, True, False, True], [True, True, True, True, True]]</t>
-  </si>
-  <si>
-    <t>[49.35, 11.82, 12.2]</t>
-  </si>
-  <si>
-    <t>[41.9, 11.39, 11.02]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">zooooooom     </t>
-  </si>
-  <si>
-    <t>[[True, True, True, True, True], [False, False, False, False, False], [False, False, False, True, True]]</t>
-  </si>
-  <si>
-    <t>[[True, True, False, True, False], [False, True, True, True, False], [False, True, True, True, False]]</t>
-  </si>
-  <si>
-    <t>[[True, False, True, True, True], [False, False, True, True, False], [False, False, False, True, False]]</t>
-  </si>
-  <si>
-    <t>[24.77, 8.8, 9.7]</t>
-  </si>
-  <si>
-    <t>[25.27, 9.49, 10.03]</t>
-  </si>
-  <si>
-    <t>[32.08, 9.67, 9.66]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DUPLO_DRONUS  </t>
-  </si>
-  <si>
-    <t>[60.17, 12.1, 12.06]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kambunji      </t>
-  </si>
-  <si>
     <t>[62.46, 21.18, 20.29]</t>
   </si>
   <si>
     <t xml:space="preserve">Dronomatized  </t>
   </si>
   <si>
-    <t>[[False, True, True, True, True], [False, True, True, True, True], [False, True, True, True, True]]</t>
-  </si>
-  <si>
     <t>[[True, False, True, True, True], [True, True, True, True, True], [True, True, True, True, True]]</t>
   </si>
   <si>
@@ -844,18 +919,6 @@
     <t>[90.62, 14.33, 14.18]</t>
   </si>
   <si>
-    <t xml:space="preserve">odermatt      </t>
-  </si>
-  <si>
-    <t>[[True, True, False, True, True], [True, True, True, True, True], [True, True, False, True, True]]</t>
-  </si>
-  <si>
-    <t>[25.26, 16.25, 16.07]</t>
-  </si>
-  <si>
-    <t>[26.17, 17.84, 16.44]</t>
-  </si>
-  <si>
     <t xml:space="preserve">Hérès         </t>
   </si>
   <si>
@@ -866,27 +929,6 @@
   </si>
   <si>
     <t>[37.12, 22.9, 22.92]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CrazyBoy      </t>
-  </si>
-  <si>
-    <t>[166.21, 15.5, 12.61]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">slowking      </t>
-  </si>
-  <si>
-    <t>[[False, True, True, False, False], [False, False, False, False, True], [False, True, True, False, True]]</t>
-  </si>
-  <si>
-    <t>[[True, False, False, False, True], [True, False, False, False, True], [False, False, False, False, True]]</t>
-  </si>
-  <si>
-    <t>[35.46, 23.9, 23.9]</t>
-  </si>
-  <si>
-    <t>[17.38, 10.38, 10.46]</t>
   </si>
   <si>
     <t>slowbutprecise</t>
@@ -1910,10 +1952,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:M71"/>
+  <dimension ref="A1:M72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="A77" sqref="A77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="17.25"/>
@@ -2026,7 +2068,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="5">
-        <v>10.8</v>
+        <v>10.52</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>13</v>
@@ -2061,7 +2103,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="5">
-        <v>10.97</v>
+        <v>10.94</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>13</v>
@@ -2131,7 +2173,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="5">
-        <v>11.88</v>
+        <v>11.55</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>13</v>
@@ -2166,7 +2208,7 @@
         <v>5</v>
       </c>
       <c r="D9" s="5">
-        <v>14.31</v>
+        <v>11.88</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>13</v>
@@ -2201,7 +2243,7 @@
         <v>5</v>
       </c>
       <c r="D10" s="5">
-        <v>14.46</v>
+        <v>14.31</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>13</v>
@@ -2236,7 +2278,7 @@
         <v>5</v>
       </c>
       <c r="D11" s="5">
-        <v>15.13</v>
+        <v>14.46</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>13</v>
@@ -2271,7 +2313,7 @@
         <v>5</v>
       </c>
       <c r="D12" s="5">
-        <v>15.2</v>
+        <v>15.13</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>13</v>
@@ -2306,7 +2348,7 @@
         <v>5</v>
       </c>
       <c r="D13" s="5">
-        <v>16.56</v>
+        <v>15.2</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>13</v>
@@ -2341,7 +2383,7 @@
         <v>5</v>
       </c>
       <c r="D14" s="5">
-        <v>16.98</v>
+        <v>16.56</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>13</v>
@@ -2376,7 +2418,7 @@
         <v>5</v>
       </c>
       <c r="D15" s="5">
-        <v>17.9</v>
+        <v>16.98</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>13</v>
@@ -2411,7 +2453,7 @@
         <v>5</v>
       </c>
       <c r="D16" s="5">
-        <v>19.59</v>
+        <v>17.27</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>13</v>
@@ -2446,7 +2488,7 @@
         <v>5</v>
       </c>
       <c r="D17" s="5">
-        <v>24.02</v>
+        <v>17.86</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>13</v>
@@ -2481,7 +2523,7 @@
         <v>5</v>
       </c>
       <c r="D18" s="5">
-        <v>45.48</v>
+        <v>19.59</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>13</v>
@@ -2513,28 +2555,28 @@
         <v>5</v>
       </c>
       <c r="C19" s="5">
-        <v>4.89</v>
+        <v>5</v>
       </c>
       <c r="D19" s="5">
-        <v>10.74</v>
+        <v>24.02</v>
       </c>
       <c r="E19" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H19" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="F19" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H19" s="5" t="s">
+      <c r="I19" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="I19" s="5" t="s">
+      <c r="J19" s="5" t="s">
         <v>76</v>
-      </c>
-      <c r="J19" s="5" t="s">
-        <v>77</v>
       </c>
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
@@ -2542,34 +2584,34 @@
     </row>
     <row r="20" spans="1:13">
       <c r="A20" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B20" s="5">
+        <v>5</v>
+      </c>
+      <c r="C20" s="5">
+        <v>5</v>
+      </c>
+      <c r="D20" s="5">
+        <v>24.5</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H20" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B20" s="5">
-        <v>5</v>
-      </c>
-      <c r="C20" s="5">
-        <v>4.78</v>
-      </c>
-      <c r="D20" s="5">
-        <v>9.18</v>
-      </c>
-      <c r="E20" s="5" t="s">
+      <c r="I20" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="F20" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H20" s="5" t="s">
+      <c r="J20" s="5" t="s">
         <v>80</v>
-      </c>
-      <c r="I20" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="J20" s="5" t="s">
-        <v>82</v>
       </c>
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
@@ -2577,34 +2619,34 @@
     </row>
     <row r="21" spans="1:13">
       <c r="A21" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B21" s="5">
+        <v>5</v>
+      </c>
+      <c r="C21" s="5">
+        <v>5</v>
+      </c>
+      <c r="D21" s="5">
+        <v>45.48</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="I21" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B21" s="5">
-        <v>5</v>
-      </c>
-      <c r="C21" s="5">
-        <v>4.78</v>
-      </c>
-      <c r="D21" s="5">
-        <v>9.88</v>
-      </c>
-      <c r="E21" s="5" t="s">
+      <c r="J21" s="5" t="s">
         <v>84</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="I21" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="J21" s="5" t="s">
-        <v>87</v>
       </c>
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
@@ -2612,34 +2654,34 @@
     </row>
     <row r="22" spans="1:13">
       <c r="A22" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22" s="5">
+        <v>5</v>
+      </c>
+      <c r="C22" s="5">
+        <v>4.89</v>
+      </c>
+      <c r="D22" s="5">
+        <v>8.53</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="I22" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B22" s="5">
-        <v>5</v>
-      </c>
-      <c r="C22" s="5">
-        <v>4.78</v>
-      </c>
-      <c r="D22" s="5">
-        <v>10.81</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G22" s="5" t="s">
+      <c r="J22" s="5" t="s">
         <v>89</v>
-      </c>
-      <c r="H22" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="I22" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="J22" s="5" t="s">
-        <v>92</v>
       </c>
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
@@ -2647,34 +2689,34 @@
     </row>
     <row r="23" spans="1:13">
       <c r="A23" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B23" s="5">
+        <v>5</v>
+      </c>
+      <c r="C23" s="5">
+        <v>4.89</v>
+      </c>
+      <c r="D23" s="5">
+        <v>8.86</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="I23" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B23" s="5">
-        <v>5</v>
-      </c>
-      <c r="C23" s="5">
-        <v>4.78</v>
-      </c>
-      <c r="D23" s="5">
-        <v>10.88</v>
-      </c>
-      <c r="E23" s="5" t="s">
+      <c r="J23" s="5" t="s">
         <v>94</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H23" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="I23" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="J23" s="5" t="s">
-        <v>97</v>
       </c>
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
@@ -2682,34 +2724,34 @@
     </row>
     <row r="24" spans="1:13">
       <c r="A24" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B24" s="5">
+        <v>5</v>
+      </c>
+      <c r="C24" s="5">
+        <v>4.89</v>
+      </c>
+      <c r="D24" s="5">
+        <v>10.84</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="I24" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="B24" s="5">
-        <v>5</v>
-      </c>
-      <c r="C24" s="5">
-        <v>4.78</v>
-      </c>
-      <c r="D24" s="5">
-        <v>11.09</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F24" s="5" t="s">
+      <c r="J24" s="5" t="s">
         <v>99</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H24" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="I24" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="J24" s="5" t="s">
-        <v>102</v>
       </c>
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
@@ -2717,34 +2759,34 @@
     </row>
     <row r="25" spans="1:13">
       <c r="A25" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B25" s="5">
+        <v>5</v>
+      </c>
+      <c r="C25" s="5">
+        <v>4.89</v>
+      </c>
+      <c r="D25" s="5">
+        <v>11.39</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="J25" s="5" t="s">
         <v>103</v>
-      </c>
-      <c r="B25" s="5">
-        <v>5</v>
-      </c>
-      <c r="C25" s="5">
-        <v>4.78</v>
-      </c>
-      <c r="D25" s="5">
-        <v>12.1</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="H25" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="I25" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="J25" s="5" t="s">
-        <v>107</v>
       </c>
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
@@ -2752,7 +2794,7 @@
     </row>
     <row r="26" spans="1:13">
       <c r="A26" s="4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B26" s="5">
         <v>5</v>
@@ -2761,10 +2803,10 @@
         <v>4.78</v>
       </c>
       <c r="D26" s="5">
-        <v>25.85</v>
+        <v>9.18</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>13</v>
@@ -2773,13 +2815,13 @@
         <v>13</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
@@ -2787,34 +2829,34 @@
     </row>
     <row r="27" spans="1:13">
       <c r="A27" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B27" s="5">
+        <v>5</v>
+      </c>
+      <c r="C27" s="5">
+        <v>4.78</v>
+      </c>
+      <c r="D27" s="5">
+        <v>9.88</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="J27" s="5" t="s">
         <v>113</v>
-      </c>
-      <c r="B27" s="5">
-        <v>5</v>
-      </c>
-      <c r="C27" s="5">
-        <v>4.67</v>
-      </c>
-      <c r="D27" s="5">
-        <v>16.12</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="I27" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="J27" s="5" t="s">
-        <v>117</v>
       </c>
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
@@ -2822,34 +2864,34 @@
     </row>
     <row r="28" spans="1:13">
       <c r="A28" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B28" s="5">
+        <v>5</v>
+      </c>
+      <c r="C28" s="5">
+        <v>4.78</v>
+      </c>
+      <c r="D28" s="5">
+        <v>10.81</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J28" s="5" t="s">
         <v>118</v>
-      </c>
-      <c r="B28" s="5">
-        <v>5</v>
-      </c>
-      <c r="C28" s="5">
-        <v>4.56</v>
-      </c>
-      <c r="D28" s="5">
-        <v>11.11</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="I28" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="J28" s="5" t="s">
-        <v>123</v>
       </c>
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
@@ -2857,34 +2899,34 @@
     </row>
     <row r="29" spans="1:13">
       <c r="A29" s="4" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B29" s="5">
         <v>5</v>
       </c>
       <c r="C29" s="5">
-        <v>3.89</v>
+        <v>4.78</v>
       </c>
       <c r="D29" s="5">
-        <v>339.11</v>
+        <v>12.1</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>13</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>125</v>
+        <v>13</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>13</v>
+        <v>120</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
@@ -2892,16 +2934,16 @@
     </row>
     <row r="30" spans="1:13">
       <c r="A30" s="4" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B30" s="5">
         <v>5</v>
       </c>
       <c r="C30" s="5">
-        <v>3.89</v>
+        <v>4.78</v>
       </c>
       <c r="D30" s="5">
-        <v>344.08</v>
+        <v>12.93</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>125</v>
@@ -2910,16 +2952,16 @@
         <v>13</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>13</v>
+        <v>125</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
@@ -2927,34 +2969,34 @@
     </row>
     <row r="31" spans="1:13">
       <c r="A31" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B31" s="5">
+        <v>5</v>
+      </c>
+      <c r="C31" s="5">
+        <v>4.67</v>
+      </c>
+      <c r="D31" s="5">
+        <v>11.2</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="H31" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="B31" s="5">
-        <v>5</v>
-      </c>
-      <c r="C31" s="5">
-        <v>3.78</v>
-      </c>
-      <c r="D31" s="5">
-        <v>342.08</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G31" s="5" t="s">
+      <c r="I31" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="H31" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="I31" s="5" t="s">
+      <c r="J31" s="5" t="s">
         <v>135</v>
-      </c>
-      <c r="J31" s="5" t="s">
-        <v>136</v>
       </c>
       <c r="K31" s="5"/>
       <c r="L31" s="5"/>
@@ -2962,34 +3004,34 @@
     </row>
     <row r="32" spans="1:13">
       <c r="A32" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B32" s="5">
+        <v>5</v>
+      </c>
+      <c r="C32" s="5">
+        <v>4.67</v>
+      </c>
+      <c r="D32" s="5">
+        <v>11.94</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G32" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="B32" s="5">
-        <v>5</v>
-      </c>
-      <c r="C32" s="5">
-        <v>2.67</v>
-      </c>
-      <c r="D32" s="5">
-        <v>12.12</v>
-      </c>
-      <c r="E32" s="5" t="s">
+      <c r="H32" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="F32" s="5" t="s">
+      <c r="I32" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="G32" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="H32" s="5" t="s">
+      <c r="J32" s="5" t="s">
         <v>140</v>
-      </c>
-      <c r="I32" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="J32" s="5" t="s">
-        <v>142</v>
       </c>
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
@@ -2997,34 +3039,34 @@
     </row>
     <row r="33" spans="1:13">
       <c r="A33" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B33" s="5">
+        <v>5</v>
+      </c>
+      <c r="C33" s="5">
+        <v>4.67</v>
+      </c>
+      <c r="D33" s="5">
+        <v>15.36</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="H33" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="B33" s="5">
-        <v>5</v>
-      </c>
-      <c r="C33" s="5">
-        <v>3</v>
-      </c>
-      <c r="D33" s="5">
-        <v>509.66</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="F33" s="5" t="s">
+      <c r="I33" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="G33" s="5" t="s">
+      <c r="J33" s="5" t="s">
         <v>145</v>
-      </c>
-      <c r="H33" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="I33" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="J33" s="5" t="s">
-        <v>148</v>
       </c>
       <c r="K33" s="5"/>
       <c r="L33" s="5"/>
@@ -3032,34 +3074,34 @@
     </row>
     <row r="34" spans="1:13">
       <c r="A34" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B34" s="5">
+        <v>5</v>
+      </c>
+      <c r="C34" s="5">
+        <v>4.67</v>
+      </c>
+      <c r="D34" s="5">
+        <v>16.12</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="I34" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="B34" s="5">
-        <v>5</v>
-      </c>
-      <c r="C34" s="5">
-        <v>2.44</v>
-      </c>
-      <c r="D34" s="5">
-        <v>6.4</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="F34" s="5" t="s">
+      <c r="J34" s="5" t="s">
         <v>150</v>
-      </c>
-      <c r="G34" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="H34" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="I34" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="J34" s="5" t="s">
-        <v>154</v>
       </c>
       <c r="K34" s="5"/>
       <c r="L34" s="5"/>
@@ -3067,34 +3109,34 @@
     </row>
     <row r="35" spans="1:13">
       <c r="A35" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B35" s="5">
+        <v>5</v>
+      </c>
+      <c r="C35" s="5">
+        <v>4</v>
+      </c>
+      <c r="D35" s="5">
+        <v>9.74</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="I35" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="B35" s="5">
-        <v>5</v>
-      </c>
-      <c r="C35" s="5">
-        <v>2.11</v>
-      </c>
-      <c r="D35" s="5">
-        <v>672.31</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="G35" s="5" t="s">
+      <c r="J35" s="5" t="s">
         <v>156</v>
-      </c>
-      <c r="H35" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="I35" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="J35" s="5" t="s">
-        <v>157</v>
       </c>
       <c r="K35" s="5"/>
       <c r="L35" s="5"/>
@@ -3102,34 +3144,34 @@
     </row>
     <row r="36" spans="1:13">
       <c r="A36" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="B36" s="5">
+        <v>5</v>
+      </c>
+      <c r="C36" s="5">
+        <v>3.89</v>
+      </c>
+      <c r="D36" s="5">
+        <v>344.08</v>
+      </c>
+      <c r="E36" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="B36" s="5">
-        <v>4.67</v>
-      </c>
-      <c r="C36" s="5">
-        <v>4.67</v>
-      </c>
-      <c r="D36" s="5">
-        <v>12.18</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>13</v>
-      </c>
       <c r="F36" s="5" t="s">
         <v>13</v>
       </c>
       <c r="G36" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H36" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="H36" s="5" t="s">
+      <c r="I36" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="I36" s="5" t="s">
+      <c r="J36" s="5" t="s">
         <v>161</v>
-      </c>
-      <c r="J36" s="5" t="s">
-        <v>162</v>
       </c>
       <c r="K36" s="5"/>
       <c r="L36" s="5"/>
@@ -3137,25 +3179,25 @@
     </row>
     <row r="37" spans="1:13">
       <c r="A37" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B37" s="5">
+        <v>5</v>
+      </c>
+      <c r="C37" s="5">
+        <v>3.33</v>
+      </c>
+      <c r="D37" s="5">
+        <v>340.05</v>
+      </c>
+      <c r="E37" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="B37" s="5">
-        <v>4.67</v>
-      </c>
-      <c r="C37" s="5">
-        <v>4.67</v>
-      </c>
-      <c r="D37" s="5">
-        <v>13.42</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>13</v>
-      </c>
       <c r="F37" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="G37" s="5" t="s">
         <v>164</v>
-      </c>
-      <c r="G37" s="5" t="s">
-        <v>13</v>
       </c>
       <c r="H37" s="5" t="s">
         <v>165</v>
@@ -3175,31 +3217,31 @@
         <v>168</v>
       </c>
       <c r="B38" s="5">
-        <v>4.67</v>
+        <v>5</v>
       </c>
       <c r="C38" s="5">
-        <v>4.67</v>
+        <v>2.67</v>
       </c>
       <c r="D38" s="5">
-        <v>23.75</v>
+        <v>12.12</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>13</v>
+        <v>169</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>13</v>
+        <v>170</v>
       </c>
       <c r="G38" s="5" t="s">
         <v>169</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="I38" s="5" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="K38" s="5"/>
       <c r="L38" s="5"/>
@@ -3207,34 +3249,34 @@
     </row>
     <row r="39" spans="1:13">
       <c r="A39" s="4" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B39" s="5">
-        <v>4.67</v>
+        <v>5</v>
       </c>
       <c r="C39" s="5">
-        <v>4.56</v>
+        <v>3</v>
       </c>
       <c r="D39" s="5">
-        <v>12.33</v>
+        <v>509.66</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>174</v>
+        <v>158</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>134</v>
+        <v>175</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I39" s="5" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="K39" s="5"/>
       <c r="L39" s="5"/>
@@ -3242,34 +3284,34 @@
     </row>
     <row r="40" spans="1:13">
       <c r="A40" s="4" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B40" s="5">
         <v>5</v>
       </c>
       <c r="C40" s="5">
-        <v>1.67</v>
+        <v>2.44</v>
       </c>
       <c r="D40" s="5">
-        <v>1000</v>
+        <v>6.4</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>125</v>
+        <v>158</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>125</v>
+        <v>181</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>125</v>
+        <v>182</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>127</v>
+        <v>183</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>127</v>
+        <v>184</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>127</v>
+        <v>185</v>
       </c>
       <c r="K40" s="5"/>
       <c r="L40" s="5"/>
@@ -3277,34 +3319,34 @@
     </row>
     <row r="41" spans="1:13">
       <c r="A41" s="4" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="B41" s="5">
         <v>5</v>
       </c>
       <c r="C41" s="5">
-        <v>1.67</v>
+        <v>2.11</v>
       </c>
       <c r="D41" s="5">
-        <v>1000</v>
+        <v>672.31</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>125</v>
+        <v>158</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>125</v>
+        <v>158</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>125</v>
+        <v>187</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>127</v>
+        <v>166</v>
       </c>
       <c r="I41" s="5" t="s">
-        <v>127</v>
+        <v>166</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>127</v>
+        <v>188</v>
       </c>
       <c r="K41" s="5"/>
       <c r="L41" s="5"/>
@@ -3312,7 +3354,7 @@
     </row>
     <row r="42" spans="1:13">
       <c r="A42" s="4" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="B42" s="5">
         <v>5</v>
@@ -3324,22 +3366,22 @@
         <v>1000</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>125</v>
+        <v>158</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>125</v>
+        <v>158</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>125</v>
+        <v>158</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>127</v>
+        <v>166</v>
       </c>
       <c r="I42" s="5" t="s">
-        <v>127</v>
+        <v>166</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>127</v>
+        <v>166</v>
       </c>
       <c r="K42" s="5"/>
       <c r="L42" s="5"/>
@@ -3347,34 +3389,34 @@
     </row>
     <row r="43" spans="1:13">
       <c r="A43" s="4" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="B43" s="5">
-        <v>4.67</v>
+        <v>5</v>
       </c>
       <c r="C43" s="5">
-        <v>3.89</v>
+        <v>1.67</v>
       </c>
       <c r="D43" s="5">
-        <v>15.92</v>
+        <v>1000</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>183</v>
+        <v>158</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>184</v>
+        <v>158</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>185</v>
+        <v>158</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>186</v>
+        <v>166</v>
       </c>
       <c r="I43" s="5" t="s">
-        <v>187</v>
+        <v>166</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>188</v>
+        <v>166</v>
       </c>
       <c r="K43" s="5"/>
       <c r="L43" s="5"/>
@@ -3382,34 +3424,34 @@
     </row>
     <row r="44" spans="1:13">
       <c r="A44" s="4" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B44" s="5">
         <v>4.67</v>
       </c>
       <c r="C44" s="5">
-        <v>3.78</v>
+        <v>4.89</v>
       </c>
       <c r="D44" s="5">
-        <v>343.65</v>
+        <v>11.17</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>13</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="G44" s="5" t="s">
         <v>13</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="I44" s="5" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="K44" s="5"/>
       <c r="L44" s="5"/>
@@ -3417,34 +3459,34 @@
     </row>
     <row r="45" spans="1:13">
       <c r="A45" s="4" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B45" s="5">
         <v>4.67</v>
       </c>
       <c r="C45" s="5">
-        <v>3.44</v>
+        <v>4.67</v>
       </c>
       <c r="D45" s="5">
-        <v>343.25</v>
+        <v>12.18</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>195</v>
+        <v>13</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>125</v>
+        <v>13</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>13</v>
+        <v>197</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>127</v>
+        <v>199</v>
       </c>
       <c r="J45" s="5" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="K45" s="5"/>
       <c r="L45" s="5"/>
@@ -3452,887 +3494,921 @@
     </row>
     <row r="46" spans="1:12">
       <c r="A46" s="4" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B46" s="5">
-        <v>4.33</v>
+        <v>4.67</v>
       </c>
       <c r="C46" s="5">
-        <v>4.33</v>
+        <v>4.67</v>
       </c>
       <c r="D46" s="5">
-        <v>10.83</v>
+        <v>13.42</v>
       </c>
       <c r="E46" s="5" t="s">
         <v>13</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="G46" s="5" t="s">
         <v>13</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="J46" s="5" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="K46" s="5"/>
       <c r="L46" s="5"/>
     </row>
     <row r="47" spans="1:12">
       <c r="A47" s="4" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="B47" s="5">
-        <v>4.33</v>
+        <v>4.67</v>
       </c>
       <c r="C47" s="5">
-        <v>4.22</v>
+        <v>4.56</v>
       </c>
       <c r="D47" s="5">
-        <v>19.98</v>
+        <v>12.33</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>74</v>
+        <v>207</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>204</v>
+        <v>125</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>13</v>
+        <v>131</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="I47" s="5" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="J47" s="5" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="K47" s="5"/>
       <c r="L47" s="5"/>
     </row>
     <row r="48" spans="1:12">
       <c r="A48" s="4" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B48" s="5">
-        <v>4.33</v>
+        <v>4.67</v>
       </c>
       <c r="C48" s="5">
-        <v>4.11</v>
+        <v>3.89</v>
       </c>
       <c r="D48" s="5">
-        <v>8.88</v>
+        <v>15.92</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>13</v>
+        <v>91</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>104</v>
+        <v>164</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="I48" s="5" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="J48" s="5" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="K48" s="5"/>
       <c r="L48" s="5"/>
     </row>
     <row r="49" spans="1:12">
       <c r="A49" s="4" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="B49" s="5">
-        <v>4.33</v>
+        <v>4.67</v>
       </c>
       <c r="C49" s="5">
         <v>3.78</v>
       </c>
       <c r="D49" s="5">
-        <v>341.58</v>
+        <v>343.65</v>
       </c>
       <c r="E49" s="5" t="s">
         <v>13</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>84</v>
+        <v>13</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="I49" s="5" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="J49" s="5" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="K49" s="5"/>
       <c r="L49" s="5"/>
     </row>
     <row r="50" spans="1:12">
       <c r="A50" s="4" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="B50" s="5">
-        <v>4.33</v>
+        <v>4.67</v>
       </c>
       <c r="C50" s="5">
-        <v>3.67</v>
+        <v>3.44</v>
       </c>
       <c r="D50" s="5">
-        <v>345.13</v>
+        <v>343.25</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>13</v>
+        <v>222</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>218</v>
+        <v>158</v>
       </c>
       <c r="G50" s="5" t="s">
         <v>13</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="I50" s="5" t="s">
-        <v>127</v>
+        <v>166</v>
       </c>
       <c r="J50" s="5" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="K50" s="5"/>
       <c r="L50" s="5"/>
     </row>
     <row r="51" spans="1:12">
       <c r="A51" s="4" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="B51" s="5">
         <v>4.33</v>
       </c>
       <c r="C51" s="5">
-        <v>2.44</v>
+        <v>4.22</v>
       </c>
       <c r="D51" s="5">
-        <v>670.05</v>
+        <v>19.98</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>222</v>
+        <v>96</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>224</v>
+        <v>13</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="I51" s="5" t="s">
-        <v>127</v>
+        <v>228</v>
       </c>
       <c r="J51" s="5" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="K51" s="5"/>
       <c r="L51" s="5"/>
     </row>
     <row r="52" spans="1:12">
       <c r="A52" s="4" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="B52" s="5">
-        <v>4</v>
+        <v>4.33</v>
       </c>
       <c r="C52" s="5">
         <v>4.11</v>
       </c>
       <c r="D52" s="5">
-        <v>14.69</v>
+        <v>8.88</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F52" s="5" t="s">
         <v>13</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>229</v>
+        <v>120</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="I52" s="5" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="J52" s="5" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="K52" s="5"/>
       <c r="L52" s="5"/>
     </row>
     <row r="53" spans="1:12">
       <c r="A53" s="4" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B53" s="5">
-        <v>4</v>
+        <v>4.33</v>
       </c>
       <c r="C53" s="5">
-        <v>4</v>
+        <v>3.78</v>
       </c>
       <c r="D53" s="5">
-        <v>13.8</v>
+        <v>341.58</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>169</v>
+        <v>13</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>164</v>
+        <v>235</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>164</v>
+        <v>110</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="I53" s="5" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="K53" s="5"/>
       <c r="L53" s="5"/>
     </row>
     <row r="54" spans="1:12">
       <c r="A54" s="4" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B54" s="5">
         <v>4.33</v>
       </c>
       <c r="C54" s="5">
-        <v>1.44</v>
+        <v>3.67</v>
       </c>
       <c r="D54" s="5">
-        <v>1000</v>
+        <v>342.7</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>238</v>
+        <v>13</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>125</v>
+        <v>13</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>127</v>
+        <v>241</v>
       </c>
       <c r="I54" s="5" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>240</v>
+        <v>166</v>
       </c>
       <c r="K54" s="5"/>
       <c r="L54" s="5"/>
     </row>
     <row r="55" spans="1:12">
       <c r="A55" s="4" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B55" s="5">
-        <v>4</v>
+        <v>4.33</v>
       </c>
       <c r="C55" s="5">
-        <v>3.44</v>
+        <v>3.67</v>
       </c>
       <c r="D55" s="5">
-        <v>340.59</v>
+        <v>345.13</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>74</v>
+        <v>13</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>13</v>
+        <v>240</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>242</v>
+        <v>13</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="I55" s="5" t="s">
-        <v>244</v>
+        <v>166</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>127</v>
+        <v>245</v>
       </c>
       <c r="K55" s="5"/>
       <c r="L55" s="5"/>
     </row>
     <row r="56" spans="1:12">
       <c r="A56" s="4" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B56" s="5">
-        <v>4</v>
+        <v>4.33</v>
       </c>
       <c r="C56" s="5">
-        <v>3.44</v>
+        <v>2.78</v>
       </c>
       <c r="D56" s="5">
-        <v>341.07</v>
+        <v>21.96</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>13</v>
+        <v>247</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="I56" s="5" t="s">
-        <v>127</v>
+        <v>251</v>
       </c>
       <c r="J56" s="5" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="K56" s="5"/>
       <c r="L56" s="5"/>
     </row>
     <row r="57" spans="1:12">
       <c r="A57" s="4" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="B57" s="5">
-        <v>4</v>
+        <v>4.33</v>
       </c>
       <c r="C57" s="5">
-        <v>2.56</v>
+        <v>2.67</v>
       </c>
       <c r="D57" s="5">
-        <v>9.56</v>
+        <v>508</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="I57" s="5" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="J57" s="5" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="K57" s="5"/>
       <c r="L57" s="5"/>
     </row>
     <row r="58" spans="1:12">
       <c r="A58" s="4" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="B58" s="5">
-        <v>4</v>
+        <v>4.33</v>
       </c>
       <c r="C58" s="5">
         <v>2.44</v>
       </c>
       <c r="D58" s="5">
-        <v>670.69</v>
+        <v>670.05</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>218</v>
+        <v>261</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>13</v>
+        <v>255</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>238</v>
+        <v>262</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>127</v>
+        <v>263</v>
       </c>
       <c r="I58" s="5" t="s">
-        <v>257</v>
+        <v>166</v>
       </c>
       <c r="J58" s="5" t="s">
-        <v>127</v>
+        <v>264</v>
       </c>
       <c r="K58" s="5"/>
       <c r="L58" s="5"/>
     </row>
     <row r="59" spans="1:12">
       <c r="A59" s="4" t="s">
-        <v>258</v>
+        <v>265</v>
       </c>
       <c r="B59" s="5">
-        <v>4</v>
+        <v>4.33</v>
       </c>
       <c r="C59" s="5">
-        <v>2.44</v>
+        <v>1.44</v>
       </c>
       <c r="D59" s="5">
-        <v>673.58</v>
+        <v>1000</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>125</v>
+        <v>266</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>13</v>
+        <v>158</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>242</v>
+        <v>266</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>127</v>
+        <v>166</v>
       </c>
       <c r="I59" s="5" t="s">
-        <v>259</v>
+        <v>267</v>
       </c>
       <c r="J59" s="5" t="s">
-        <v>127</v>
+        <v>268</v>
       </c>
       <c r="K59" s="5"/>
       <c r="L59" s="5"/>
     </row>
     <row r="60" spans="1:12">
       <c r="A60" s="4" t="s">
-        <v>260</v>
+        <v>269</v>
       </c>
       <c r="B60" s="5">
-        <v>3.67</v>
+        <v>4</v>
       </c>
       <c r="C60" s="5">
-        <v>4.11</v>
+        <v>4</v>
       </c>
       <c r="D60" s="5">
-        <v>12.97</v>
+        <v>13.34</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>261</v>
+        <v>270</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>262</v>
+        <v>202</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>263</v>
+        <v>202</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>264</v>
+        <v>271</v>
       </c>
       <c r="I60" s="5" t="s">
-        <v>265</v>
+        <v>272</v>
       </c>
       <c r="J60" s="5" t="s">
-        <v>266</v>
+        <v>273</v>
       </c>
       <c r="K60" s="5"/>
       <c r="L60" s="5"/>
     </row>
     <row r="61" spans="1:12">
       <c r="A61" s="4" t="s">
-        <v>267</v>
+        <v>274</v>
       </c>
       <c r="B61" s="5">
-        <v>3.67</v>
+        <v>4</v>
       </c>
       <c r="C61" s="5">
-        <v>3.22</v>
+        <v>2.56</v>
       </c>
       <c r="D61" s="5">
-        <v>341.07</v>
+        <v>9.56</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>268</v>
+        <v>275</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>13</v>
+        <v>276</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>127</v>
+        <v>278</v>
       </c>
       <c r="I61" s="5" t="s">
-        <v>270</v>
+        <v>279</v>
       </c>
       <c r="J61" s="5" t="s">
-        <v>271</v>
+        <v>280</v>
       </c>
       <c r="K61" s="5"/>
       <c r="L61" s="5"/>
     </row>
     <row r="62" spans="1:12">
       <c r="A62" s="4" t="s">
-        <v>272</v>
+        <v>281</v>
       </c>
       <c r="B62" s="5">
-        <v>3.33</v>
+        <v>4</v>
       </c>
       <c r="C62" s="5">
-        <v>3.33</v>
+        <v>2.44</v>
       </c>
       <c r="D62" s="5">
-        <v>343.64</v>
+        <v>670.69</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>13</v>
+        <v>240</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>273</v>
+        <v>13</v>
       </c>
       <c r="G62" s="5" t="s">
-        <v>13</v>
+        <v>266</v>
       </c>
       <c r="H62" s="5" t="s">
-        <v>274</v>
+        <v>166</v>
       </c>
       <c r="I62" s="5" t="s">
-        <v>127</v>
+        <v>282</v>
       </c>
       <c r="J62" s="5" t="s">
-        <v>275</v>
+        <v>166</v>
       </c>
       <c r="K62" s="5"/>
       <c r="L62" s="5"/>
     </row>
     <row r="63" spans="1:12">
       <c r="A63" s="4" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="B63" s="5">
-        <v>3.33</v>
+        <v>4</v>
       </c>
       <c r="C63" s="5">
-        <v>3.22</v>
+        <v>2.44</v>
       </c>
       <c r="D63" s="5">
-        <v>344.43</v>
+        <v>673.58</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>13</v>
+        <v>158</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>277</v>
+        <v>13</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>268</v>
+        <v>284</v>
       </c>
       <c r="H63" s="5" t="s">
-        <v>278</v>
+        <v>166</v>
       </c>
       <c r="I63" s="5" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="J63" s="5" t="s">
-        <v>127</v>
+        <v>166</v>
       </c>
       <c r="K63" s="5"/>
       <c r="L63" s="5"/>
     </row>
     <row r="64" spans="1:12">
       <c r="A64" s="4" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="B64" s="5">
-        <v>3.33</v>
+        <v>3.67</v>
       </c>
       <c r="C64" s="5">
-        <v>3.22</v>
+        <v>4.11</v>
       </c>
       <c r="D64" s="5">
-        <v>348.85</v>
+        <v>12.97</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>268</v>
+        <v>287</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>13</v>
+        <v>288</v>
       </c>
       <c r="H64" s="5" t="s">
-        <v>282</v>
+        <v>289</v>
       </c>
       <c r="I64" s="5" t="s">
-        <v>127</v>
+        <v>290</v>
       </c>
       <c r="J64" s="5" t="s">
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="K64" s="5"/>
       <c r="L64" s="5"/>
     </row>
     <row r="65" spans="1:12">
       <c r="A65" s="4" t="s">
-        <v>284</v>
+        <v>292</v>
       </c>
       <c r="B65" s="5">
-        <v>3</v>
+        <v>3.67</v>
       </c>
       <c r="C65" s="5">
-        <v>1.89</v>
+        <v>3.22</v>
       </c>
       <c r="D65" s="5">
-        <v>671.35</v>
+        <v>341.07</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>169</v>
+        <v>293</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>268</v>
+        <v>13</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>238</v>
+        <v>294</v>
       </c>
       <c r="H65" s="5" t="s">
-        <v>285</v>
+        <v>166</v>
       </c>
       <c r="I65" s="5" t="s">
-        <v>127</v>
+        <v>295</v>
       </c>
       <c r="J65" s="5" t="s">
-        <v>127</v>
+        <v>296</v>
       </c>
       <c r="K65" s="5"/>
       <c r="L65" s="5"/>
     </row>
     <row r="66" spans="1:12">
       <c r="A66" s="4" t="s">
-        <v>286</v>
+        <v>297</v>
       </c>
       <c r="B66" s="5">
-        <v>2</v>
+        <v>3.33</v>
       </c>
       <c r="C66" s="5">
-        <v>1.44</v>
+        <v>3.33</v>
       </c>
       <c r="D66" s="5">
-        <v>344.77</v>
+        <v>343.64</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>287</v>
+        <v>13</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>288</v>
+        <v>298</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>242</v>
+        <v>13</v>
       </c>
       <c r="H66" s="5" t="s">
-        <v>289</v>
+        <v>299</v>
       </c>
       <c r="I66" s="5" t="s">
-        <v>290</v>
+        <v>166</v>
       </c>
       <c r="J66" s="5" t="s">
-        <v>127</v>
+        <v>300</v>
       </c>
       <c r="K66" s="5"/>
       <c r="L66" s="5"/>
     </row>
     <row r="67" spans="1:12">
       <c r="A67" s="4" t="s">
-        <v>291</v>
+        <v>301</v>
       </c>
       <c r="B67" s="5">
-        <v>2</v>
+        <v>3.33</v>
       </c>
       <c r="C67" s="5">
-        <v>0.67</v>
+        <v>3.22</v>
       </c>
       <c r="D67" s="5">
-        <v>1000</v>
+        <v>348.85</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>242</v>
+        <v>302</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>218</v>
+        <v>293</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>268</v>
+        <v>13</v>
       </c>
       <c r="H67" s="5" t="s">
-        <v>127</v>
+        <v>303</v>
       </c>
       <c r="I67" s="5" t="s">
-        <v>127</v>
+        <v>166</v>
       </c>
       <c r="J67" s="5" t="s">
-        <v>127</v>
+        <v>304</v>
       </c>
       <c r="K67" s="5"/>
       <c r="L67" s="5"/>
     </row>
     <row r="68" spans="1:12">
       <c r="A68" s="4" t="s">
-        <v>292</v>
+        <v>305</v>
       </c>
       <c r="B68" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C68" s="5">
-        <v>0.67</v>
+        <v>1</v>
       </c>
       <c r="D68" s="5">
         <v>1000</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>268</v>
+        <v>158</v>
       </c>
       <c r="F68" s="5" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="G68" s="5" t="s">
         <v>293</v>
       </c>
       <c r="H68" s="5" t="s">
-        <v>127</v>
+        <v>166</v>
       </c>
       <c r="I68" s="5" t="s">
-        <v>127</v>
+        <v>166</v>
       </c>
       <c r="J68" s="5" t="s">
-        <v>127</v>
+        <v>166</v>
       </c>
       <c r="K68" s="5"/>
       <c r="L68" s="5"/>
     </row>
     <row r="69" spans="1:12">
       <c r="A69" s="4" t="s">
-        <v>294</v>
+        <v>306</v>
       </c>
       <c r="B69" s="5">
-        <v>1.67</v>
+        <v>2</v>
       </c>
       <c r="C69" s="5">
-        <v>0.78</v>
+        <v>0.67</v>
       </c>
       <c r="D69" s="5">
-        <v>687.35</v>
+        <v>1000</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>268</v>
+        <v>293</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>295</v>
+        <v>284</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>296</v>
+        <v>307</v>
       </c>
       <c r="H69" s="5" t="s">
-        <v>127</v>
+        <v>166</v>
       </c>
       <c r="I69" s="5" t="s">
-        <v>297</v>
+        <v>166</v>
       </c>
       <c r="J69" s="5" t="s">
-        <v>127</v>
+        <v>166</v>
       </c>
       <c r="K69" s="5"/>
       <c r="L69" s="5"/>
     </row>
     <row r="70" spans="1:12">
       <c r="A70" s="4" t="s">
-        <v>298</v>
+        <v>308</v>
       </c>
       <c r="B70" s="5">
         <v>1.67</v>
       </c>
       <c r="C70" s="5">
-        <v>0.56</v>
+        <v>0.78</v>
       </c>
       <c r="D70" s="5">
-        <v>1000</v>
+        <v>687.35</v>
       </c>
       <c r="E70" s="5" t="s">
-        <v>268</v>
+        <v>293</v>
       </c>
       <c r="F70" s="5" t="s">
-        <v>268</v>
+        <v>309</v>
       </c>
       <c r="G70" s="5" t="s">
-        <v>218</v>
+        <v>310</v>
       </c>
       <c r="H70" s="5" t="s">
-        <v>127</v>
+        <v>166</v>
       </c>
       <c r="I70" s="5" t="s">
-        <v>127</v>
+        <v>311</v>
       </c>
       <c r="J70" s="5" t="s">
-        <v>127</v>
+        <v>166</v>
       </c>
       <c r="K70" s="5"/>
       <c r="L70" s="5"/>
     </row>
     <row r="71" spans="1:12">
       <c r="A71" s="4" t="s">
-        <v>299</v>
+        <v>312</v>
       </c>
       <c r="B71" s="5">
-        <v>0</v>
+        <v>1.67</v>
       </c>
       <c r="C71" s="5">
-        <v>0</v>
+        <v>0.56</v>
       </c>
       <c r="D71" s="5">
         <v>1000</v>
       </c>
       <c r="E71" s="5" t="s">
-        <v>273</v>
+        <v>293</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>273</v>
+        <v>293</v>
       </c>
       <c r="G71" s="5" t="s">
-        <v>273</v>
+        <v>240</v>
       </c>
       <c r="H71" s="5" t="s">
-        <v>127</v>
+        <v>166</v>
       </c>
       <c r="I71" s="5" t="s">
-        <v>127</v>
+        <v>166</v>
       </c>
       <c r="J71" s="5" t="s">
-        <v>127</v>
+        <v>166</v>
       </c>
       <c r="K71" s="5"/>
       <c r="L71" s="5"/>
+    </row>
+    <row r="72" spans="1:12">
+      <c r="A72" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="B72" s="5">
+        <v>0</v>
+      </c>
+      <c r="C72" s="5">
+        <v>0</v>
+      </c>
+      <c r="D72" s="5">
+        <v>1000</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="F72" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="G72" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="H72" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="I72" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="J72" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="K72" s="5"/>
+      <c r="L72" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>